<commit_message>
Update Excel string resources
</commit_message>
<xml_diff>
--- a/ErgoLux/localization/Finnish (fi-FI) translation.xlsx
+++ b/ErgoLux/localization/Finnish (fi-FI) translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthurit\source\repos\ErgoLux\ErgoLux\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D298696F-2DD0-4234-A89A-1A0344F40F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14860DBA-7944-4C33-80B8-828BC591A107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{51C6AD1F-7C4A-41E1-BFD1-D5AAE4E918C7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="389">
   <si>
     <t>Key</t>
   </si>
@@ -1159,7 +1159,64 @@
     <t>Save data</t>
   </si>
   <si>
-    <t>fi-FI</t>
+    <t>Finnish (fi-FI)</t>
+  </si>
+  <si>
+    <t>strFileDlgFileName</t>
+  </si>
+  <si>
+    <t>Plots' context menu</t>
+  </si>
+  <si>
+    <t>Plot.png</t>
+  </si>
+  <si>
+    <t>strFileDlgFilter</t>
+  </si>
+  <si>
+    <t>PNG Files (*.png)|*.png;*.png|JPG Files (*.jpg, *.jpeg)|*.jpg;*.jpeg|BMP Files (*.bmp)|*.bmp;*.bmp|All files (*.*)|*.*</t>
+  </si>
+  <si>
+    <t>strMenuCopy</t>
+  </si>
+  <si>
+    <t>Copy image</t>
+  </si>
+  <si>
+    <t>strMenuCrossHair</t>
+  </si>
+  <si>
+    <t>Show crosshair</t>
+  </si>
+  <si>
+    <t>strMenuDetach</t>
+  </si>
+  <si>
+    <t>Detach legend</t>
+  </si>
+  <si>
+    <t>strMenuHelp</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>strMenuOpen</t>
+  </si>
+  <si>
+    <t>Open in new window</t>
+  </si>
+  <si>
+    <t>strMenuSave</t>
+  </si>
+  <si>
+    <t>Save image as...</t>
+  </si>
+  <si>
+    <t>strMenuZoom</t>
+  </si>
+  <si>
+    <t>Zoom to fit data</t>
   </si>
 </sst>
 </file>
@@ -1246,8 +1303,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DD7C0AF-0A3F-45E4-9CF3-D3036D280B58}" name="Tabla13" displayName="Tabla13" ref="B2:E194" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="B2:E194" xr:uid="{64291C3F-0D0C-4C57-A011-4795D69358B3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DD7C0AF-0A3F-45E4-9CF3-D3036D280B58}" name="Tabla13" displayName="Tabla13" ref="B2:E203" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="B2:E203" xr:uid="{64291C3F-0D0C-4C57-A011-4795D69358B3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:E169">
     <sortCondition ref="B2:B169"/>
   </sortState>
@@ -1255,7 +1312,7 @@
     <tableColumn id="1" xr3:uid="{15B209E7-880B-40F3-8D04-E1E0C18F3997}" name="Key" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{1492BE55-1C7C-4C02-9979-85AD6633F924}" name="Comment" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{3A0B826D-ACD0-42A2-BC11-CDF70F40C5E5}" name="English" dataDxfId="1"/>
-    <tableColumn id="31" xr3:uid="{482B5252-4A88-4C9D-8D6A-67323FB06C35}" name="fi-FI" dataDxfId="0"/>
+    <tableColumn id="31" xr3:uid="{482B5252-4A88-4C9D-8D6A-67323FB06C35}" name="Finnish (fi-FI)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3556,7 +3613,77 @@
       </c>
       <c r="E194" s="1"/>
     </row>
+    <row r="195" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B195" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="E195" s="1"/>
+    </row>
+    <row r="196" spans="2:28" ht="45" x14ac:dyDescent="0.25">
+      <c r="B196" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="E196" s="1"/>
+    </row>
+    <row r="197" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B197" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="E197" s="1"/>
+    </row>
+    <row r="198" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B198" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D198" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E198" s="1"/>
+    </row>
+    <row r="199" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B199" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E199" s="1"/>
+    </row>
     <row r="200" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B200" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="E200" s="1"/>
       <c r="F200" s="2"/>
       <c r="L200" s="2"/>
       <c r="N200" s="2"/>
@@ -3565,7 +3692,29 @@
       <c r="X200" s="2"/>
       <c r="Z200" s="2"/>
     </row>
+    <row r="201" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B201" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="E201" s="1"/>
+    </row>
     <row r="202" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B202" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="E202" s="1"/>
       <c r="F202" s="2"/>
       <c r="H202" s="2"/>
       <c r="J202" s="2"/>
@@ -3578,6 +3727,18 @@
       <c r="X202" s="2"/>
       <c r="Z202" s="2"/>
       <c r="AB202" s="2"/>
+    </row>
+    <row r="203" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B203" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="E203" s="1"/>
     </row>
     <row r="229" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F229" s="2"/>

</xml_diff>